<commit_message>
size table results implemented
</commit_message>
<xml_diff>
--- a/slim_gsgp/comparison_results.xlsx
+++ b/slim_gsgp/comparison_results.xlsx
@@ -16,10 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,13 +35,17 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
     </font>
     <font>
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="102">
+  <fills count="163">
     <fill>
       <patternFill/>
     </fill>
@@ -55,6 +60,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+        <bgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00D9E1F2"/>
         <bgColor rgb="00D9E1F2"/>
       </patternFill>
@@ -645,6 +656,366 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFF7F7"/>
         <bgColor rgb="00FFF7F7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF4F4"/>
+        <bgColor rgb="00FFF4F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE6E6"/>
+        <bgColor rgb="00FFE6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B4F3B4"/>
+        <bgColor rgb="00B4F3B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFDCDC"/>
+        <bgColor rgb="00FFDCDC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFDDDD"/>
+        <bgColor rgb="00FFDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F3FDF3"/>
+        <bgColor rgb="00F3FDF3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F6FDF6"/>
+        <bgColor rgb="00F6FDF6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F1FCF1"/>
+        <bgColor rgb="00F1FCF1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFAFA"/>
+        <bgColor rgb="00FFFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B2F3B2"/>
+        <bgColor rgb="00B2F3B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A5F1A5"/>
+        <bgColor rgb="00A5F1A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF1F1"/>
+        <bgColor rgb="00FFF1F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DEF9DE"/>
+        <bgColor rgb="00DEF9DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6FBE6"/>
+        <bgColor rgb="00E6FBE6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDF9DD"/>
+        <bgColor rgb="00DDF9DD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ECFCEC"/>
+        <bgColor rgb="00ECFCEC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A4F1A4"/>
+        <bgColor rgb="00A4F1A4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FBFEFB"/>
+        <bgColor rgb="00FBFEFB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DCF9DC"/>
+        <bgColor rgb="00DCF9DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8FDF8"/>
+        <bgColor rgb="00F8FDF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4D4D"/>
+        <bgColor rgb="00FF4D4D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF5656"/>
+        <bgColor rgb="00FF5656"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF7B7B"/>
+        <bgColor rgb="00FF7B7B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF9696"/>
+        <bgColor rgb="00FF9696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA8A8"/>
+        <bgColor rgb="00FFA8A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B7F4B7"/>
+        <bgColor rgb="00B7F4B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFBFBF"/>
+        <bgColor rgb="00FFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFDADA"/>
+        <bgColor rgb="00FFDADA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE7E7"/>
+        <bgColor rgb="00FFE7E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC9C9"/>
+        <bgColor rgb="00FFC9C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEEEE"/>
+        <bgColor rgb="00FFEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCCCC"/>
+        <bgColor rgb="00FFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEBEB"/>
+        <bgColor rgb="00FFEBEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F2FDF2"/>
+        <bgColor rgb="00F2FDF2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF3F3"/>
+        <bgColor rgb="00FFF3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00AFF2AF"/>
+        <bgColor rgb="00AFF2AF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF0F0"/>
+        <bgColor rgb="00FFF0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CFF7CF"/>
+        <bgColor rgb="00CFF7CF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E4FBE4"/>
+        <bgColor rgb="00E4FBE4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E5FBE5"/>
+        <bgColor rgb="00E5FBE5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0097EF97"/>
+        <bgColor rgb="0097EF97"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E2FAE2"/>
+        <bgColor rgb="00E2FAE2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C2F5C2"/>
+        <bgColor rgb="00C2F5C2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0098EF98"/>
+        <bgColor rgb="0098EF98"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4FDF4"/>
+        <bgColor rgb="00F4FDF4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0096EF96"/>
+        <bgColor rgb="0096EF96"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFD9D9"/>
+        <bgColor rgb="00FFD9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF5F5"/>
+        <bgColor rgb="00FFF5F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF7171"/>
+        <bgColor rgb="00FF7171"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA2A2"/>
+        <bgColor rgb="00FFA2A2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF8282"/>
+        <bgColor rgb="00FF8282"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BDF4BD"/>
+        <bgColor rgb="00BDF4BD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFCFCF"/>
+        <bgColor rgb="00FFCFCF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEDED"/>
+        <bgColor rgb="00FFEDED"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF7676"/>
+        <bgColor rgb="00FF7676"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7FBE7"/>
+        <bgColor rgb="00E7FBE7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF8181"/>
+        <bgColor rgb="00FF8181"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEFEF"/>
+        <bgColor rgb="00FFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE5E5"/>
+        <bgColor rgb="00FFE5E5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B8F4B8"/>
+        <bgColor rgb="00B8F4B8"/>
       </patternFill>
     </fill>
   </fills>
@@ -666,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -675,15 +1046,15 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -973,6 +1344,342 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="101" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="102" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="84" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="103" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="90" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="64" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="104" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="98" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="105" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="106" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="107" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="108" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="109" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="39" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="76" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="72" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="110" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="111" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="112" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="113" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="18" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="102" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="50" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="114" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="81" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="82" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="115" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="116" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="117" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="118" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="43" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="119" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="83" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="99" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="120" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="121" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="122" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="123" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="124" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="125" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="126" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="127" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="47" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="128" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="58" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="129" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="130" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="131" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="132" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="133" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="134" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="135" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="136" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="137" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="138" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="139" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="23" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="140" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="92" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="31" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="24" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="141" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="32" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="142" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="143" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="144" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="145" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="80" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="146" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="66" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="147" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="89" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="75" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="67" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="148" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="149" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="150" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="74" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="151" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="152" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="153" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="29" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="154" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="65" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="155" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="156" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="157" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="158" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="159" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="96" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="85" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="40" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="19" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="77" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="28" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="160" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="161" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="162" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="71" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="49" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="57" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1340,7 +2047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1405,7 +2112,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Dataset 1 airfoil</t>
+          <t>PERFORMANCE - TEST FITNESS</t>
         </is>
       </c>
       <c r="B2" s="3" t="n"/>
@@ -1420,1498 +2127,3083 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
+          <t>Dataset 1 airfoil</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B4" s="6" t="n">
         <v>51.58366</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C4" s="7" t="n">
         <v>23.33073</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D4" s="7" t="n">
         <v>5.44271</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E4" s="7" t="n">
         <v>5.3321</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F4" s="8" t="n">
         <v>67.16248</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G4" s="7" t="n">
         <v>5.5513</v>
       </c>
-      <c r="H3" s="7" t="n">
+      <c r="H4" s="8" t="n">
         <v>67.16248</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I4" s="7" t="n">
         <v>5.5513</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B4" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <v>50.49002</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="C5" s="7" t="n">
         <v>6.17759</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D5" s="7" t="n">
         <v>5.39968</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E5" s="7" t="n">
         <v>5.048</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F5" s="7" t="n">
         <v>11.72197</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G5" s="7" t="n">
         <v>5.49476</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H5" s="7" t="n">
         <v>11.91436</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I5" s="7" t="n">
         <v>5.4906</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <v>49.77869</v>
       </c>
-      <c r="C5" s="6" t="n">
+      <c r="C6" s="7" t="n">
         <v>4.82857</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D6" s="7" t="n">
         <v>5.37385</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E6" s="7" t="n">
         <v>4.95534</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F6" s="7" t="n">
         <v>5.29925</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G6" s="7" t="n">
         <v>5.45337</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H6" s="7" t="n">
         <v>5.29925</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I6" s="7" t="n">
         <v>5.44963</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 2 bike_sharing</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="n"/>
-      <c r="I6" s="3" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
+          <t>Dataset 2 bike_sharing</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="3" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
+      <c r="I7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B8" s="6" t="n">
         <v>971.6932399999999</v>
       </c>
-      <c r="C7" s="8" t="n">
+      <c r="C8" s="9" t="n">
         <v>682.53388</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <v>449.29437</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E8" s="7" t="n">
         <v>322.51454</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F8" s="10" t="n">
         <v>975.7971700000001</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <v>450.57209</v>
       </c>
-      <c r="H7" s="10" t="n">
+      <c r="H8" s="11" t="n">
         <v>973.2086</v>
       </c>
-      <c r="I7" s="6" t="n">
+      <c r="I8" s="7" t="n">
         <v>450.57199</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B9" s="6" t="n">
         <v>970.60237</v>
       </c>
-      <c r="C8" s="11" t="n">
+      <c r="C9" s="12" t="n">
         <v>630.54644</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D9" s="7" t="n">
         <v>448.68596</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E9" s="7" t="n">
         <v>296.12761</v>
       </c>
-      <c r="F8" s="12" t="n">
+      <c r="F9" s="13" t="n">
         <v>751.38075</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G9" s="7" t="n">
         <v>449.66007</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H9" s="13" t="n">
         <v>749.50472</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I9" s="7" t="n">
         <v>449.53246</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B10" s="6" t="n">
         <v>969.94817</v>
       </c>
-      <c r="C9" s="13" t="n">
+      <c r="C10" s="14" t="n">
         <v>604.79182</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D10" s="7" t="n">
         <v>448.38704</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E10" s="7" t="n">
         <v>283.75204</v>
       </c>
-      <c r="F9" s="14" t="n">
+      <c r="F10" s="15" t="n">
         <v>611.1578</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G10" s="7" t="n">
         <v>448.95808</v>
       </c>
-      <c r="H9" s="14" t="n">
+      <c r="H10" s="15" t="n">
         <v>611.1578</v>
       </c>
-      <c r="I9" s="6" t="n">
+      <c r="I10" s="7" t="n">
         <v>448.89562</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 3 bioavailability</t>
-        </is>
-      </c>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="3" t="n"/>
-      <c r="D10" s="3" t="n"/>
-      <c r="E10" s="3" t="n"/>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
-      <c r="H10" s="3" t="n"/>
-      <c r="I10" s="3" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
+          <t>Dataset 3 bioavailability</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="n"/>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="3" t="n"/>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="3" t="n"/>
+      <c r="I11" s="3" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B12" s="6" t="n">
         <v>49.9188</v>
       </c>
-      <c r="C11" s="15" t="n">
+      <c r="C12" s="16" t="n">
         <v>40.84623</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D12" s="17" t="n">
         <v>30.19743</v>
       </c>
-      <c r="E11" s="16" t="n">
+      <c r="E12" s="17" t="n">
         <v>30.30966</v>
       </c>
-      <c r="F11" s="17" t="n">
+      <c r="F12" s="18" t="n">
         <v>54.02734</v>
       </c>
-      <c r="G11" s="18" t="n">
+      <c r="G12" s="19" t="n">
         <v>30.02608</v>
       </c>
-      <c r="H11" s="17" t="n">
+      <c r="H12" s="18" t="n">
         <v>54.02734</v>
       </c>
-      <c r="I11" s="18" t="n">
+      <c r="I12" s="19" t="n">
         <v>30.08082</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+    <row r="13">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B13" s="6" t="n">
         <v>49.00977</v>
       </c>
-      <c r="C12" s="18" t="n">
+      <c r="C13" s="19" t="n">
         <v>29.4582</v>
       </c>
-      <c r="D12" s="19" t="n">
+      <c r="D13" s="20" t="n">
         <v>30.19548</v>
       </c>
-      <c r="E12" s="13" t="n">
+      <c r="E13" s="14" t="n">
         <v>30.47309</v>
       </c>
-      <c r="F12" s="14" t="n">
+      <c r="F13" s="15" t="n">
         <v>30.69939</v>
       </c>
-      <c r="G12" s="19" t="n">
+      <c r="G13" s="20" t="n">
         <v>30.20468</v>
       </c>
-      <c r="H12" s="14" t="n">
+      <c r="H13" s="15" t="n">
         <v>30.69939</v>
       </c>
-      <c r="I12" s="20" t="n">
+      <c r="I13" s="21" t="n">
         <v>30.00804</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B14" s="6" t="n">
         <v>48.38265</v>
       </c>
-      <c r="C13" s="19" t="n">
+      <c r="C14" s="20" t="n">
         <v>29.82236</v>
       </c>
-      <c r="D13" s="14" t="n">
+      <c r="D14" s="15" t="n">
         <v>30.43734</v>
       </c>
-      <c r="E13" s="21" t="n">
+      <c r="E14" s="22" t="n">
         <v>30.56269</v>
       </c>
-      <c r="F13" s="16" t="n">
+      <c r="F14" s="17" t="n">
         <v>29.28927</v>
       </c>
-      <c r="G13" s="14" t="n">
+      <c r="G14" s="15" t="n">
         <v>30.38595</v>
       </c>
-      <c r="H13" s="16" t="n">
+      <c r="H14" s="17" t="n">
         <v>29.28927</v>
       </c>
-      <c r="I13" s="14" t="n">
+      <c r="I14" s="15" t="n">
         <v>30.31073</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 5 breast_cancer</t>
-        </is>
-      </c>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" s="3" t="n"/>
-      <c r="D14" s="3" t="n"/>
-      <c r="E14" s="3" t="n"/>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
-      <c r="H14" s="3" t="n"/>
-      <c r="I14" s="3" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
+          <t>Dataset 5 breast_cancer</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="n"/>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="n"/>
+      <c r="E15" s="3" t="n"/>
+      <c r="F15" s="3" t="n"/>
+      <c r="G15" s="3" t="n"/>
+      <c r="H15" s="3" t="n"/>
+      <c r="I15" s="3" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B16" s="6" t="n">
         <v>0.54137</v>
       </c>
-      <c r="C15" s="22" t="n">
+      <c r="C16" s="23" t="n">
         <v>0.42729</v>
       </c>
-      <c r="D15" s="23" t="n">
+      <c r="D16" s="24" t="n">
         <v>0.27315</v>
       </c>
-      <c r="E15" s="6" t="n">
+      <c r="E16" s="7" t="n">
         <v>0.26921</v>
       </c>
-      <c r="F15" s="24" t="n">
+      <c r="F16" s="25" t="n">
         <v>0.52418</v>
       </c>
-      <c r="G15" s="25" t="n">
+      <c r="G16" s="26" t="n">
         <v>0.29714</v>
       </c>
-      <c r="H15" s="24" t="n">
+      <c r="H16" s="25" t="n">
         <v>0.52418</v>
       </c>
-      <c r="I15" s="25" t="n">
+      <c r="I16" s="26" t="n">
         <v>0.29736</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B17" s="6" t="n">
         <v>0.36687</v>
       </c>
-      <c r="C16" s="26" t="n">
+      <c r="C17" s="27" t="n">
         <v>0.27399</v>
       </c>
-      <c r="D16" s="27" t="n">
+      <c r="D17" s="28" t="n">
         <v>0.25128</v>
       </c>
-      <c r="E16" s="28" t="n">
+      <c r="E17" s="29" t="n">
         <v>0.25605</v>
       </c>
-      <c r="F16" s="29" t="n">
+      <c r="F17" s="30" t="n">
         <v>0.30507</v>
       </c>
-      <c r="G16" s="30" t="n">
+      <c r="G17" s="31" t="n">
         <v>0.26506</v>
       </c>
-      <c r="H16" s="29" t="n">
+      <c r="H17" s="30" t="n">
         <v>0.30507</v>
       </c>
-      <c r="I16" s="30" t="n">
+      <c r="I17" s="31" t="n">
         <v>0.26603</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n">
+      <c r="B18" s="6" t="n">
         <v>0.31465</v>
       </c>
-      <c r="C17" s="31" t="n">
+      <c r="C18" s="32" t="n">
         <v>0.26349</v>
       </c>
-      <c r="D17" s="22" t="n">
+      <c r="D18" s="23" t="n">
         <v>0.24857</v>
       </c>
-      <c r="E17" s="32" t="n">
+      <c r="E18" s="33" t="n">
         <v>0.25343</v>
       </c>
-      <c r="F17" s="33" t="n">
+      <c r="F18" s="34" t="n">
         <v>0.27541</v>
       </c>
-      <c r="G17" s="34" t="n">
+      <c r="G18" s="35" t="n">
         <v>0.25509</v>
       </c>
-      <c r="H17" s="33" t="n">
+      <c r="H18" s="34" t="n">
         <v>0.27541</v>
       </c>
-      <c r="I17" s="34" t="n">
+      <c r="I18" s="35" t="n">
         <v>0.25508</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 6 concrete_slump</t>
-        </is>
-      </c>
-      <c r="B18" s="3" t="n"/>
-      <c r="C18" s="3" t="n"/>
-      <c r="D18" s="3" t="n"/>
-      <c r="E18" s="3" t="n"/>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="n"/>
-      <c r="H18" s="3" t="n"/>
-      <c r="I18" s="3" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
+          <t>Dataset 6 concrete_slump</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="n"/>
+      <c r="C19" s="3" t="n"/>
+      <c r="D19" s="3" t="n"/>
+      <c r="E19" s="3" t="n"/>
+      <c r="F19" s="3" t="n"/>
+      <c r="G19" s="3" t="n"/>
+      <c r="H19" s="3" t="n"/>
+      <c r="I19" s="3" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B19" s="5" t="n">
+      <c r="B20" s="6" t="n">
         <v>10.9548</v>
       </c>
-      <c r="C19" s="35" t="n">
+      <c r="C20" s="36" t="n">
         <v>9.934060000000001</v>
       </c>
-      <c r="D19" s="26" t="n">
+      <c r="D20" s="27" t="n">
         <v>8.187580000000001</v>
       </c>
-      <c r="E19" s="35" t="n">
+      <c r="E20" s="36" t="n">
         <v>9.95682</v>
       </c>
-      <c r="F19" s="36" t="n">
+      <c r="F20" s="37" t="n">
         <v>13.34257</v>
       </c>
-      <c r="G19" s="37" t="n">
+      <c r="G20" s="38" t="n">
         <v>8.250019999999999</v>
       </c>
-      <c r="H19" s="36" t="n">
+      <c r="H20" s="37" t="n">
         <v>13.34257</v>
       </c>
-      <c r="I19" s="38" t="n">
+      <c r="I20" s="39" t="n">
         <v>8.224909999999999</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="4" t="inlineStr">
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B20" s="5" t="n">
+      <c r="B21" s="6" t="n">
         <v>10.60387</v>
       </c>
-      <c r="C20" s="39" t="n">
+      <c r="C21" s="40" t="n">
         <v>7.80095</v>
       </c>
-      <c r="D20" s="26" t="n">
+      <c r="D21" s="27" t="n">
         <v>7.91517</v>
       </c>
-      <c r="E20" s="40" t="n">
+      <c r="E21" s="41" t="n">
         <v>9.93473</v>
       </c>
-      <c r="F20" s="41" t="n">
+      <c r="F21" s="42" t="n">
         <v>8.76885</v>
       </c>
-      <c r="G20" s="42" t="n">
+      <c r="G21" s="43" t="n">
         <v>8.14411</v>
       </c>
-      <c r="H20" s="41" t="n">
+      <c r="H21" s="42" t="n">
         <v>8.78131</v>
       </c>
-      <c r="I20" s="12" t="n">
+      <c r="I21" s="13" t="n">
         <v>8.185689999999999</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="4" t="inlineStr">
+    <row r="22">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B21" s="5" t="n">
+      <c r="B22" s="6" t="n">
         <v>10.39858</v>
       </c>
-      <c r="C21" s="39" t="n">
+      <c r="C22" s="40" t="n">
         <v>7.67514</v>
       </c>
-      <c r="D21" s="43" t="n">
+      <c r="D22" s="44" t="n">
         <v>7.91244</v>
       </c>
-      <c r="E21" s="44" t="n">
+      <c r="E22" s="45" t="n">
         <v>9.936439999999999</v>
       </c>
-      <c r="F21" s="42" t="n">
+      <c r="F22" s="43" t="n">
         <v>7.99648</v>
       </c>
-      <c r="G21" s="45" t="n">
+      <c r="G22" s="46" t="n">
         <v>8.12025</v>
       </c>
-      <c r="H21" s="42" t="n">
+      <c r="H22" s="43" t="n">
         <v>7.99648</v>
       </c>
-      <c r="I21" s="45" t="n">
+      <c r="I22" s="46" t="n">
         <v>8.12365</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 7 concrete_strength</t>
-        </is>
-      </c>
-      <c r="B22" s="3" t="n"/>
-      <c r="C22" s="3" t="n"/>
-      <c r="D22" s="3" t="n"/>
-      <c r="E22" s="3" t="n"/>
-      <c r="F22" s="3" t="n"/>
-      <c r="G22" s="3" t="n"/>
-      <c r="H22" s="3" t="n"/>
-      <c r="I22" s="3" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
+          <t>Dataset 7 concrete_strength</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="n"/>
+      <c r="C23" s="3" t="n"/>
+      <c r="D23" s="3" t="n"/>
+      <c r="E23" s="3" t="n"/>
+      <c r="F23" s="3" t="n"/>
+      <c r="G23" s="3" t="n"/>
+      <c r="H23" s="3" t="n"/>
+      <c r="I23" s="3" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n">
+      <c r="B24" s="6" t="n">
         <v>22.99887</v>
       </c>
-      <c r="C23" s="46" t="n">
+      <c r="C24" s="47" t="n">
         <v>15.87307</v>
       </c>
-      <c r="D23" s="6" t="n">
+      <c r="D24" s="7" t="n">
         <v>11.55726</v>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E24" s="7" t="n">
         <v>11.07097</v>
       </c>
-      <c r="F23" s="47" t="n">
+      <c r="F24" s="48" t="n">
         <v>26.75151</v>
       </c>
-      <c r="G23" s="48" t="n">
+      <c r="G24" s="49" t="n">
         <v>13.41887</v>
       </c>
-      <c r="H23" s="47" t="n">
+      <c r="H24" s="48" t="n">
         <v>26.75151</v>
       </c>
-      <c r="I23" s="49" t="n">
+      <c r="I24" s="50" t="n">
         <v>13.35493</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="4" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n">
+      <c r="B25" s="6" t="n">
         <v>22.16967</v>
       </c>
-      <c r="C24" s="6" t="n">
+      <c r="C25" s="7" t="n">
         <v>9.83128</v>
       </c>
-      <c r="D24" s="6" t="n">
+      <c r="D25" s="7" t="n">
         <v>10.50817</v>
       </c>
-      <c r="E24" s="6" t="n">
+      <c r="E25" s="7" t="n">
         <v>9.269080000000001</v>
       </c>
-      <c r="F24" s="20" t="n">
+      <c r="F25" s="21" t="n">
         <v>13.57534</v>
       </c>
-      <c r="G24" s="23" t="n">
+      <c r="G25" s="24" t="n">
         <v>11.26173</v>
       </c>
-      <c r="H24" s="19" t="n">
+      <c r="H25" s="20" t="n">
         <v>13.63266</v>
       </c>
-      <c r="I24" s="50" t="n">
+      <c r="I25" s="51" t="n">
         <v>11.33615</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="4" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n">
+      <c r="B26" s="6" t="n">
         <v>21.72682</v>
       </c>
-      <c r="C25" s="6" t="n">
+      <c r="C26" s="7" t="n">
         <v>8.58924</v>
       </c>
-      <c r="D25" s="6" t="n">
+      <c r="D26" s="7" t="n">
         <v>10.23339</v>
       </c>
-      <c r="E25" s="6" t="n">
+      <c r="E26" s="7" t="n">
         <v>8.875730000000001</v>
       </c>
-      <c r="F25" s="6" t="n">
+      <c r="F26" s="7" t="n">
         <v>9.21442</v>
       </c>
-      <c r="G25" s="6" t="n">
+      <c r="G26" s="7" t="n">
         <v>10.42694</v>
       </c>
-      <c r="H25" s="6" t="n">
+      <c r="H26" s="7" t="n">
         <v>9.21442</v>
       </c>
-      <c r="I25" s="6" t="n">
+      <c r="I26" s="7" t="n">
         <v>10.34252</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 8 diabetes</t>
-        </is>
-      </c>
-      <c r="B26" s="3" t="n"/>
-      <c r="C26" s="3" t="n"/>
-      <c r="D26" s="3" t="n"/>
-      <c r="E26" s="3" t="n"/>
-      <c r="F26" s="3" t="n"/>
-      <c r="G26" s="3" t="n"/>
-      <c r="H26" s="3" t="n"/>
-      <c r="I26" s="3" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
+          <t>Dataset 8 diabetes</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="n"/>
+      <c r="C27" s="3" t="n"/>
+      <c r="D27" s="3" t="n"/>
+      <c r="E27" s="3" t="n"/>
+      <c r="F27" s="3" t="n"/>
+      <c r="G27" s="3" t="n"/>
+      <c r="H27" s="3" t="n"/>
+      <c r="I27" s="3" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B27" s="5" t="n">
+      <c r="B28" s="6" t="n">
         <v>156.08804</v>
       </c>
-      <c r="C27" s="23" t="n">
+      <c r="C28" s="24" t="n">
         <v>79.44725</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D28" s="7" t="n">
         <v>60.22883</v>
       </c>
-      <c r="E27" s="6" t="n">
+      <c r="E28" s="7" t="n">
         <v>61.49329</v>
       </c>
-      <c r="F27" s="51" t="n">
+      <c r="F28" s="52" t="n">
         <v>154.55045</v>
       </c>
-      <c r="G27" s="6" t="n">
+      <c r="G28" s="7" t="n">
         <v>62.65541</v>
       </c>
-      <c r="H27" s="51" t="n">
+      <c r="H28" s="52" t="n">
         <v>154.55045</v>
       </c>
-      <c r="I27" s="6" t="n">
+      <c r="I28" s="7" t="n">
         <v>62.65541</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="4" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B29" s="6" t="n">
         <v>154.88839</v>
       </c>
-      <c r="C28" s="6" t="n">
+      <c r="C29" s="7" t="n">
         <v>71.57778</v>
       </c>
-      <c r="D28" s="6" t="n">
+      <c r="D29" s="7" t="n">
         <v>58.78443</v>
       </c>
-      <c r="E28" s="6" t="n">
+      <c r="E29" s="7" t="n">
         <v>58.40838</v>
       </c>
-      <c r="F28" s="52" t="n">
+      <c r="F29" s="53" t="n">
         <v>81.03989</v>
       </c>
-      <c r="G28" s="6" t="n">
+      <c r="G29" s="7" t="n">
         <v>59.39253</v>
       </c>
-      <c r="H28" s="53" t="n">
+      <c r="H29" s="54" t="n">
         <v>81.77663</v>
       </c>
-      <c r="I28" s="6" t="n">
+      <c r="I29" s="7" t="n">
         <v>58.91464</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="4" t="inlineStr">
+    <row r="30">
+      <c r="A30" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B29" s="5" t="n">
+      <c r="B30" s="6" t="n">
         <v>154.08919</v>
       </c>
-      <c r="C29" s="6" t="n">
+      <c r="C30" s="7" t="n">
         <v>70.03449999999999</v>
       </c>
-      <c r="D29" s="6" t="n">
+      <c r="D30" s="7" t="n">
         <v>58.25503</v>
       </c>
-      <c r="E29" s="6" t="n">
+      <c r="E30" s="7" t="n">
         <v>57.58964</v>
       </c>
-      <c r="F29" s="6" t="n">
+      <c r="F30" s="7" t="n">
         <v>73.70976</v>
       </c>
-      <c r="G29" s="6" t="n">
+      <c r="G30" s="7" t="n">
         <v>57.9234</v>
       </c>
-      <c r="H29" s="6" t="n">
+      <c r="H30" s="7" t="n">
         <v>73.70976</v>
       </c>
-      <c r="I29" s="6" t="n">
+      <c r="I30" s="7" t="n">
         <v>57.93185</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 9 efficiency_cooling</t>
-        </is>
-      </c>
-      <c r="B30" s="3" t="n"/>
-      <c r="C30" s="3" t="n"/>
-      <c r="D30" s="3" t="n"/>
-      <c r="E30" s="3" t="n"/>
-      <c r="F30" s="3" t="n"/>
-      <c r="G30" s="3" t="n"/>
-      <c r="H30" s="3" t="n"/>
-      <c r="I30" s="3" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
+          <t>Dataset 9 efficiency_cooling</t>
+        </is>
+      </c>
+      <c r="B31" s="3" t="n"/>
+      <c r="C31" s="3" t="n"/>
+      <c r="D31" s="3" t="n"/>
+      <c r="E31" s="3" t="n"/>
+      <c r="F31" s="3" t="n"/>
+      <c r="G31" s="3" t="n"/>
+      <c r="H31" s="3" t="n"/>
+      <c r="I31" s="3" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B31" s="5" t="n">
+      <c r="B32" s="6" t="n">
         <v>8.11303</v>
       </c>
-      <c r="C31" s="54" t="n">
+      <c r="C32" s="55" t="n">
         <v>4.48805</v>
       </c>
-      <c r="D31" s="6" t="n">
+      <c r="D32" s="7" t="n">
         <v>3.71105</v>
       </c>
-      <c r="E31" s="6" t="n">
+      <c r="E32" s="7" t="n">
         <v>3.66672</v>
       </c>
-      <c r="F31" s="55" t="n">
+      <c r="F32" s="56" t="n">
         <v>11.07758</v>
       </c>
-      <c r="G31" s="6" t="n">
+      <c r="G32" s="7" t="n">
         <v>4.01559</v>
       </c>
-      <c r="H31" s="55" t="n">
+      <c r="H32" s="56" t="n">
         <v>11.07758</v>
       </c>
-      <c r="I31" s="6" t="n">
+      <c r="I32" s="7" t="n">
         <v>4.05867</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B32" s="5" t="n">
+      <c r="B33" s="6" t="n">
         <v>7.58892</v>
       </c>
-      <c r="C32" s="6" t="n">
+      <c r="C33" s="7" t="n">
         <v>3.66402</v>
       </c>
-      <c r="D32" s="6" t="n">
+      <c r="D33" s="7" t="n">
         <v>3.55884</v>
       </c>
-      <c r="E32" s="6" t="n">
+      <c r="E33" s="7" t="n">
         <v>3.4125</v>
       </c>
-      <c r="F32" s="20" t="n">
+      <c r="F33" s="21" t="n">
         <v>4.63091</v>
       </c>
-      <c r="G32" s="6" t="n">
+      <c r="G33" s="7" t="n">
         <v>3.68179</v>
       </c>
-      <c r="H32" s="16" t="n">
+      <c r="H33" s="17" t="n">
         <v>4.60735</v>
       </c>
-      <c r="I32" s="6" t="n">
+      <c r="I33" s="7" t="n">
         <v>3.65599</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="4" t="inlineStr">
+    <row r="34">
+      <c r="A34" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B33" s="5" t="n">
+      <c r="B34" s="6" t="n">
         <v>7.30619</v>
       </c>
-      <c r="C33" s="6" t="n">
+      <c r="C34" s="7" t="n">
         <v>3.5356</v>
       </c>
-      <c r="D33" s="6" t="n">
+      <c r="D34" s="7" t="n">
         <v>3.52352</v>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E34" s="7" t="n">
         <v>3.3697</v>
       </c>
-      <c r="F33" s="6" t="n">
+      <c r="F34" s="7" t="n">
         <v>3.64905</v>
       </c>
-      <c r="G33" s="6" t="n">
+      <c r="G34" s="7" t="n">
         <v>3.56183</v>
       </c>
-      <c r="H33" s="6" t="n">
+      <c r="H34" s="7" t="n">
         <v>3.64905</v>
       </c>
-      <c r="I33" s="6" t="n">
+      <c r="I34" s="7" t="n">
         <v>3.54255</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 10 efficiency_heating</t>
-        </is>
-      </c>
-      <c r="B34" s="3" t="n"/>
-      <c r="C34" s="3" t="n"/>
-      <c r="D34" s="3" t="n"/>
-      <c r="E34" s="3" t="n"/>
-      <c r="F34" s="3" t="n"/>
-      <c r="G34" s="3" t="n"/>
-      <c r="H34" s="3" t="n"/>
-      <c r="I34" s="3" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
+          <t>Dataset 10 efficiency_heating</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="n"/>
+      <c r="C35" s="3" t="n"/>
+      <c r="D35" s="3" t="n"/>
+      <c r="E35" s="3" t="n"/>
+      <c r="F35" s="3" t="n"/>
+      <c r="G35" s="3" t="n"/>
+      <c r="H35" s="3" t="n"/>
+      <c r="I35" s="3" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B35" s="5" t="n">
+      <c r="B36" s="6" t="n">
         <v>7.5216</v>
       </c>
-      <c r="C35" s="56" t="n">
+      <c r="C36" s="57" t="n">
         <v>5.74214</v>
       </c>
-      <c r="D35" s="6" t="n">
+      <c r="D36" s="7" t="n">
         <v>3.64571</v>
       </c>
-      <c r="E35" s="6" t="n">
+      <c r="E36" s="7" t="n">
         <v>3.6938</v>
       </c>
-      <c r="F35" s="57" t="n">
+      <c r="F36" s="58" t="n">
         <v>10.14764</v>
       </c>
-      <c r="G35" s="58" t="n">
+      <c r="G36" s="59" t="n">
         <v>4.26729</v>
       </c>
-      <c r="H35" s="57" t="n">
+      <c r="H36" s="58" t="n">
         <v>10.14764</v>
       </c>
-      <c r="I35" s="59" t="n">
+      <c r="I36" s="60" t="n">
         <v>4.2788</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="4" t="inlineStr">
+    <row r="37">
+      <c r="A37" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B36" s="5" t="n">
+      <c r="B37" s="6" t="n">
         <v>7.08955</v>
       </c>
-      <c r="C36" s="6" t="n">
+      <c r="C37" s="7" t="n">
         <v>3.46467</v>
       </c>
-      <c r="D36" s="6" t="n">
+      <c r="D37" s="7" t="n">
         <v>3.35834</v>
       </c>
-      <c r="E36" s="6" t="n">
+      <c r="E37" s="7" t="n">
         <v>3.05673</v>
       </c>
-      <c r="F36" s="60" t="n">
+      <c r="F37" s="61" t="n">
         <v>4.75459</v>
       </c>
-      <c r="G36" s="61" t="n">
+      <c r="G37" s="62" t="n">
         <v>3.68151</v>
       </c>
-      <c r="H36" s="62" t="n">
+      <c r="H37" s="63" t="n">
         <v>4.58944</v>
       </c>
-      <c r="I36" s="52" t="n">
+      <c r="I37" s="53" t="n">
         <v>3.7109</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="4" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B37" s="5" t="n">
+      <c r="B38" s="6" t="n">
         <v>6.86537</v>
       </c>
-      <c r="C37" s="6" t="n">
+      <c r="C38" s="7" t="n">
         <v>3.30218</v>
       </c>
-      <c r="D37" s="6" t="n">
+      <c r="D38" s="7" t="n">
         <v>3.27716</v>
       </c>
-      <c r="E37" s="6" t="n">
+      <c r="E38" s="7" t="n">
         <v>2.96911</v>
       </c>
-      <c r="F37" s="6" t="n">
+      <c r="F38" s="7" t="n">
         <v>3.42546</v>
       </c>
-      <c r="G37" s="23" t="n">
+      <c r="G38" s="24" t="n">
         <v>3.48953</v>
       </c>
-      <c r="H37" s="6" t="n">
+      <c r="H38" s="7" t="n">
         <v>3.42546</v>
       </c>
-      <c r="I37" s="23" t="n">
+      <c r="I38" s="24" t="n">
         <v>3.48069</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 11 forest_fires</t>
-        </is>
-      </c>
-      <c r="B38" s="3" t="n"/>
-      <c r="C38" s="3" t="n"/>
-      <c r="D38" s="3" t="n"/>
-      <c r="E38" s="3" t="n"/>
-      <c r="F38" s="3" t="n"/>
-      <c r="G38" s="3" t="n"/>
-      <c r="H38" s="3" t="n"/>
-      <c r="I38" s="3" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
+          <t>Dataset 11 forest_fires</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="n"/>
+      <c r="C39" s="3" t="n"/>
+      <c r="D39" s="3" t="n"/>
+      <c r="E39" s="3" t="n"/>
+      <c r="F39" s="3" t="n"/>
+      <c r="G39" s="3" t="n"/>
+      <c r="H39" s="3" t="n"/>
+      <c r="I39" s="3" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B39" s="5" t="n">
+      <c r="B40" s="6" t="n">
         <v>1.43257</v>
       </c>
-      <c r="C39" s="63" t="n">
+      <c r="C40" s="64" t="n">
         <v>1.69364</v>
       </c>
-      <c r="D39" s="51" t="n">
+      <c r="D40" s="52" t="n">
         <v>1.41702</v>
       </c>
-      <c r="E39" s="51" t="n">
+      <c r="E40" s="52" t="n">
         <v>1.41961</v>
       </c>
-      <c r="F39" s="64" t="n">
+      <c r="F40" s="65" t="n">
         <v>1.64749</v>
       </c>
-      <c r="G39" s="65" t="n">
+      <c r="G40" s="66" t="n">
         <v>1.39883</v>
       </c>
-      <c r="H39" s="64" t="n">
+      <c r="H40" s="65" t="n">
         <v>1.64749</v>
       </c>
-      <c r="I39" s="65" t="n">
+      <c r="I40" s="66" t="n">
         <v>1.40002</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="4" t="inlineStr">
+    <row r="41">
+      <c r="A41" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B40" s="5" t="n">
+      <c r="B41" s="6" t="n">
         <v>1.41149</v>
       </c>
-      <c r="C40" s="66" t="n">
+      <c r="C41" s="67" t="n">
         <v>1.67275</v>
       </c>
-      <c r="D40" s="67" t="n">
+      <c r="D41" s="68" t="n">
         <v>1.42804</v>
       </c>
-      <c r="E40" s="68" t="n">
+      <c r="E41" s="69" t="n">
         <v>1.4397</v>
       </c>
-      <c r="F40" s="69" t="n">
+      <c r="F41" s="70" t="n">
         <v>1.64814</v>
       </c>
-      <c r="G40" s="70" t="n">
+      <c r="G41" s="71" t="n">
         <v>1.40883</v>
       </c>
-      <c r="H40" s="69" t="n">
+      <c r="H41" s="70" t="n">
         <v>1.64814</v>
       </c>
-      <c r="I40" s="70" t="n">
+      <c r="I41" s="71" t="n">
         <v>1.4061</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="4" t="inlineStr">
+    <row r="42">
+      <c r="A42" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B41" s="5" t="n">
+      <c r="B42" s="6" t="n">
         <v>1.41038</v>
       </c>
-      <c r="C41" s="71" t="n">
+      <c r="C42" s="72" t="n">
         <v>1.68071</v>
       </c>
-      <c r="D41" s="72" t="n">
+      <c r="D42" s="73" t="n">
         <v>1.43436</v>
       </c>
-      <c r="E41" s="73" t="n">
+      <c r="E42" s="74" t="n">
         <v>1.44671</v>
       </c>
-      <c r="F41" s="74" t="n">
+      <c r="F42" s="75" t="n">
         <v>1.65955</v>
       </c>
-      <c r="G41" s="75" t="n">
+      <c r="G42" s="76" t="n">
         <v>1.42003</v>
       </c>
-      <c r="H41" s="74" t="n">
+      <c r="H42" s="75" t="n">
         <v>1.65955</v>
       </c>
-      <c r="I41" s="75" t="n">
+      <c r="I42" s="76" t="n">
         <v>1.42021</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 12 istanbul</t>
-        </is>
-      </c>
-      <c r="B42" s="3" t="n"/>
-      <c r="C42" s="3" t="n"/>
-      <c r="D42" s="3" t="n"/>
-      <c r="E42" s="3" t="n"/>
-      <c r="F42" s="3" t="n"/>
-      <c r="G42" s="3" t="n"/>
-      <c r="H42" s="3" t="n"/>
-      <c r="I42" s="3" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
+          <t>Dataset 12 istanbul</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="n"/>
+      <c r="C43" s="3" t="n"/>
+      <c r="D43" s="3" t="n"/>
+      <c r="E43" s="3" t="n"/>
+      <c r="F43" s="3" t="n"/>
+      <c r="G43" s="3" t="n"/>
+      <c r="H43" s="3" t="n"/>
+      <c r="I43" s="3" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B43" s="5" t="n">
+      <c r="B44" s="6" t="n">
         <v>0.01626</v>
       </c>
-      <c r="C43" s="76" t="n">
+      <c r="C44" s="77" t="n">
         <v>0.01512</v>
       </c>
-      <c r="D43" s="77" t="n">
+      <c r="D44" s="78" t="n">
         <v>0.01466</v>
       </c>
-      <c r="E43" s="78" t="n">
+      <c r="E44" s="79" t="n">
         <v>0.01459</v>
       </c>
-      <c r="F43" s="70" t="n">
+      <c r="F44" s="71" t="n">
         <v>0.01621</v>
       </c>
-      <c r="G43" s="35" t="n">
+      <c r="G44" s="36" t="n">
         <v>0.01473</v>
       </c>
-      <c r="H43" s="70" t="n">
+      <c r="H44" s="71" t="n">
         <v>0.01621</v>
       </c>
-      <c r="I43" s="79" t="n">
+      <c r="I44" s="80" t="n">
         <v>0.01485</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="4" t="inlineStr">
+    <row r="45">
+      <c r="A45" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B44" s="5" t="n">
+      <c r="B45" s="6" t="n">
         <v>0.01572</v>
       </c>
-      <c r="C44" s="40" t="n">
+      <c r="C45" s="41" t="n">
         <v>0.01468</v>
       </c>
-      <c r="D44" s="80" t="n">
+      <c r="D45" s="81" t="n">
         <v>0.01433</v>
       </c>
-      <c r="E44" s="81" t="n">
+      <c r="E45" s="82" t="n">
         <v>0.01448</v>
       </c>
-      <c r="F44" s="82" t="n">
+      <c r="F45" s="83" t="n">
         <v>0.01455</v>
       </c>
-      <c r="G44" s="35" t="n">
+      <c r="G45" s="36" t="n">
         <v>0.01425</v>
       </c>
-      <c r="H44" s="82" t="n">
+      <c r="H45" s="83" t="n">
         <v>0.01456</v>
       </c>
-      <c r="I44" s="79" t="n">
+      <c r="I45" s="80" t="n">
         <v>0.01434</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="4" t="inlineStr">
+    <row r="46">
+      <c r="A46" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B45" s="5" t="n">
+      <c r="B46" s="6" t="n">
         <v>0.01462</v>
       </c>
-      <c r="C45" s="83" t="n">
+      <c r="C46" s="84" t="n">
         <v>0.01477</v>
       </c>
-      <c r="D45" s="65" t="n">
+      <c r="D46" s="66" t="n">
         <v>0.01425</v>
       </c>
-      <c r="E45" s="84" t="n">
+      <c r="E46" s="85" t="n">
         <v>0.0145</v>
       </c>
-      <c r="F45" s="70" t="n">
+      <c r="F46" s="71" t="n">
         <v>0.01457</v>
       </c>
-      <c r="G45" s="85" t="n">
+      <c r="G46" s="86" t="n">
         <v>0.01422</v>
       </c>
-      <c r="H45" s="70" t="n">
+      <c r="H46" s="71" t="n">
         <v>0.01457</v>
       </c>
-      <c r="I45" s="86" t="n">
+      <c r="I46" s="87" t="n">
         <v>0.01432</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 13 parkinson_updrs</t>
-        </is>
-      </c>
-      <c r="B46" s="3" t="n"/>
-      <c r="C46" s="3" t="n"/>
-      <c r="D46" s="3" t="n"/>
-      <c r="E46" s="3" t="n"/>
-      <c r="F46" s="3" t="n"/>
-      <c r="G46" s="3" t="n"/>
-      <c r="H46" s="3" t="n"/>
-      <c r="I46" s="3" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
+          <t>Dataset 13 parkinson_updrs</t>
+        </is>
+      </c>
+      <c r="B47" s="3" t="n"/>
+      <c r="C47" s="3" t="n"/>
+      <c r="D47" s="3" t="n"/>
+      <c r="E47" s="3" t="n"/>
+      <c r="F47" s="3" t="n"/>
+      <c r="G47" s="3" t="n"/>
+      <c r="H47" s="3" t="n"/>
+      <c r="I47" s="3" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B47" s="5" t="n">
+      <c r="B48" s="6" t="n">
         <v>12.61269</v>
       </c>
-      <c r="C47" s="74" t="n">
+      <c r="C48" s="75" t="n">
         <v>14.85123</v>
       </c>
-      <c r="D47" s="87" t="n">
+      <c r="D48" s="88" t="n">
         <v>10.10083</v>
       </c>
-      <c r="E47" s="88" t="n">
+      <c r="E48" s="89" t="n">
         <v>10.03231</v>
       </c>
-      <c r="F47" s="89" t="n">
+      <c r="F48" s="90" t="n">
         <v>16.36131</v>
       </c>
-      <c r="G47" s="32" t="n">
+      <c r="G48" s="33" t="n">
         <v>10.16786</v>
       </c>
-      <c r="H47" s="89" t="n">
+      <c r="H48" s="90" t="n">
         <v>16.36131</v>
       </c>
-      <c r="I47" s="32" t="n">
+      <c r="I48" s="33" t="n">
         <v>10.16786</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="4" t="inlineStr">
+    <row r="49">
+      <c r="A49" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B48" s="5" t="n">
+      <c r="B49" s="6" t="n">
         <v>12.33529</v>
       </c>
-      <c r="C48" s="29" t="n">
+      <c r="C49" s="30" t="n">
         <v>10.26647</v>
       </c>
-      <c r="D48" s="15" t="n">
+      <c r="D49" s="16" t="n">
         <v>10.07893</v>
       </c>
-      <c r="E48" s="34" t="n">
+      <c r="E49" s="35" t="n">
         <v>9.958629999999999</v>
       </c>
-      <c r="F48" s="90" t="n">
+      <c r="F49" s="91" t="n">
         <v>10.64115</v>
       </c>
-      <c r="G48" s="91" t="n">
+      <c r="G49" s="92" t="n">
         <v>10.12573</v>
       </c>
-      <c r="H48" s="92" t="n">
+      <c r="H49" s="93" t="n">
         <v>10.66898</v>
       </c>
-      <c r="I48" s="91" t="n">
+      <c r="I49" s="92" t="n">
         <v>10.13004</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="4" t="inlineStr">
+    <row r="50">
+      <c r="A50" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B49" s="5" t="n">
+      <c r="B50" s="6" t="n">
         <v>12.17768</v>
       </c>
-      <c r="C49" s="31" t="n">
+      <c r="C50" s="32" t="n">
         <v>10.19441</v>
       </c>
-      <c r="D49" s="41" t="n">
+      <c r="D50" s="42" t="n">
         <v>10.06395</v>
       </c>
-      <c r="E49" s="15" t="n">
+      <c r="E50" s="16" t="n">
         <v>9.929209999999999</v>
       </c>
-      <c r="F49" s="93" t="n">
+      <c r="F50" s="94" t="n">
         <v>10.22274</v>
       </c>
-      <c r="G49" s="29" t="n">
+      <c r="G50" s="30" t="n">
         <v>10.10271</v>
       </c>
-      <c r="H49" s="93" t="n">
+      <c r="H50" s="94" t="n">
         <v>10.22274</v>
       </c>
-      <c r="I49" s="29" t="n">
+      <c r="I50" s="30" t="n">
         <v>10.10095</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 14 ppb</t>
-        </is>
-      </c>
-      <c r="B50" s="3" t="n"/>
-      <c r="C50" s="3" t="n"/>
-      <c r="D50" s="3" t="n"/>
-      <c r="E50" s="3" t="n"/>
-      <c r="F50" s="3" t="n"/>
-      <c r="G50" s="3" t="n"/>
-      <c r="H50" s="3" t="n"/>
-      <c r="I50" s="3" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
+          <t>Dataset 14 ppb</t>
+        </is>
+      </c>
+      <c r="B51" s="3" t="n"/>
+      <c r="C51" s="3" t="n"/>
+      <c r="D51" s="3" t="n"/>
+      <c r="E51" s="3" t="n"/>
+      <c r="F51" s="3" t="n"/>
+      <c r="G51" s="3" t="n"/>
+      <c r="H51" s="3" t="n"/>
+      <c r="I51" s="3" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B51" s="5" t="n">
+      <c r="B52" s="6" t="n">
         <v>39.69858</v>
       </c>
-      <c r="C51" s="92" t="n">
+      <c r="C52" s="93" t="n">
         <v>34.34471</v>
       </c>
-      <c r="D51" s="93" t="n">
+      <c r="D52" s="94" t="n">
         <v>33.29498</v>
       </c>
-      <c r="E51" s="88" t="n">
+      <c r="E52" s="89" t="n">
         <v>31.54396</v>
       </c>
-      <c r="F51" s="94" t="n">
+      <c r="F52" s="95" t="n">
         <v>44.6434</v>
       </c>
-      <c r="G51" s="95" t="n">
+      <c r="G52" s="96" t="n">
         <v>31.47374</v>
       </c>
-      <c r="H51" s="94" t="n">
+      <c r="H52" s="95" t="n">
         <v>44.6434</v>
       </c>
-      <c r="I51" s="95" t="n">
+      <c r="I52" s="96" t="n">
         <v>31.52066</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="4" t="inlineStr">
+    <row r="53">
+      <c r="A53" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B52" s="5" t="n">
+      <c r="B53" s="6" t="n">
         <v>39.28653</v>
       </c>
-      <c r="C52" s="38" t="n">
+      <c r="C53" s="39" t="n">
         <v>29.43047</v>
       </c>
-      <c r="D52" s="96" t="n">
+      <c r="D53" s="97" t="n">
         <v>33.75612</v>
       </c>
-      <c r="E52" s="87" t="n">
+      <c r="E53" s="88" t="n">
         <v>31.33168</v>
       </c>
-      <c r="F52" s="22" t="n">
+      <c r="F53" s="23" t="n">
         <v>31.03134</v>
       </c>
-      <c r="G52" s="97" t="n">
+      <c r="G53" s="98" t="n">
         <v>32.02607</v>
       </c>
-      <c r="H52" s="22" t="n">
+      <c r="H53" s="23" t="n">
         <v>31.067</v>
       </c>
-      <c r="I52" s="98" t="n">
+      <c r="I53" s="99" t="n">
         <v>32.38255</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="4" t="inlineStr">
+    <row r="54">
+      <c r="A54" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B53" s="5" t="n">
+      <c r="B54" s="6" t="n">
         <v>38.83346</v>
       </c>
-      <c r="C53" s="56" t="n">
+      <c r="C54" s="57" t="n">
         <v>29.57433</v>
       </c>
-      <c r="D53" s="99" t="n">
+      <c r="D54" s="100" t="n">
         <v>34.25611</v>
       </c>
-      <c r="E53" s="95" t="n">
+      <c r="E54" s="96" t="n">
         <v>30.83682</v>
       </c>
-      <c r="F53" s="88" t="n">
+      <c r="F54" s="89" t="n">
         <v>30.93703</v>
       </c>
-      <c r="G53" s="100" t="n">
+      <c r="G54" s="101" t="n">
         <v>33.18373</v>
       </c>
-      <c r="H53" s="88" t="n">
+      <c r="H54" s="89" t="n">
         <v>30.93703</v>
       </c>
-      <c r="I53" s="93" t="n">
+      <c r="I54" s="94" t="n">
         <v>32.64378</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="2" t="inlineStr">
-        <is>
-          <t>Dataset 15 resid_build_sale_price</t>
-        </is>
-      </c>
-      <c r="B54" s="3" t="n"/>
-      <c r="C54" s="3" t="n"/>
-      <c r="D54" s="3" t="n"/>
-      <c r="E54" s="3" t="n"/>
-      <c r="F54" s="3" t="n"/>
-      <c r="G54" s="3" t="n"/>
-      <c r="H54" s="3" t="n"/>
-      <c r="I54" s="3" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
+          <t>Dataset 15 resid_build_sale_price</t>
+        </is>
+      </c>
+      <c r="B55" s="3" t="n"/>
+      <c r="C55" s="3" t="n"/>
+      <c r="D55" s="3" t="n"/>
+      <c r="E55" s="3" t="n"/>
+      <c r="F55" s="3" t="n"/>
+      <c r="G55" s="3" t="n"/>
+      <c r="H55" s="3" t="n"/>
+      <c r="I55" s="3" t="n"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="5" t="inlineStr">
+        <is>
           <t>Smallest</t>
         </is>
       </c>
-      <c r="B55" s="5" t="n">
+      <c r="B56" s="6" t="n">
         <v>129.09692</v>
       </c>
-      <c r="C55" s="101" t="n">
+      <c r="C56" s="102" t="n">
         <v>94.83167</v>
       </c>
-      <c r="D55" s="102" t="n">
+      <c r="D56" s="103" t="n">
         <v>92.76797999999999</v>
       </c>
-      <c r="E55" s="20" t="n">
+      <c r="E56" s="21" t="n">
         <v>78.66724000000001</v>
       </c>
-      <c r="F55" s="103" t="n">
+      <c r="F56" s="104" t="n">
         <v>132.10529</v>
       </c>
-      <c r="G55" s="30" t="n">
+      <c r="G56" s="31" t="n">
         <v>93.30089</v>
       </c>
-      <c r="H55" s="103" t="n">
+      <c r="H56" s="104" t="n">
         <v>132.10529</v>
       </c>
-      <c r="I55" s="30" t="n">
+      <c r="I56" s="31" t="n">
         <v>93.30089</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="4" t="inlineStr">
+    <row r="57">
+      <c r="A57" s="5" t="inlineStr">
         <is>
           <t>Best normalized</t>
         </is>
       </c>
-      <c r="B56" s="5" t="n">
+      <c r="B57" s="6" t="n">
         <v>128.51271</v>
       </c>
-      <c r="C56" s="21" t="n">
+      <c r="C57" s="22" t="n">
         <v>81.47093</v>
       </c>
-      <c r="D56" s="102" t="n">
+      <c r="D57" s="103" t="n">
         <v>92.53823</v>
       </c>
-      <c r="E56" s="48" t="n">
+      <c r="E57" s="49" t="n">
         <v>74.98727</v>
       </c>
-      <c r="F56" s="37" t="n">
+      <c r="F57" s="38" t="n">
         <v>96.98033</v>
       </c>
-      <c r="G56" s="30" t="n">
+      <c r="G57" s="31" t="n">
         <v>92.88059</v>
       </c>
-      <c r="H56" s="38" t="n">
+      <c r="H57" s="39" t="n">
         <v>96.3895</v>
       </c>
-      <c r="I56" s="30" t="n">
+      <c r="I57" s="31" t="n">
         <v>92.72686</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="4" t="inlineStr">
+    <row r="58">
+      <c r="A58" s="5" t="inlineStr">
         <is>
           <t>Best fitness</t>
         </is>
       </c>
-      <c r="B57" s="5" t="n">
+      <c r="B58" s="6" t="n">
         <v>128.08286</v>
       </c>
-      <c r="C57" s="13" t="n">
+      <c r="C58" s="14" t="n">
         <v>79.67587</v>
       </c>
-      <c r="D57" s="30" t="n">
+      <c r="D58" s="31" t="n">
         <v>92.43795</v>
       </c>
-      <c r="E57" s="49" t="n">
+      <c r="E58" s="50" t="n">
         <v>74.38186</v>
       </c>
-      <c r="F57" s="11" t="n">
+      <c r="F58" s="12" t="n">
         <v>83.55507</v>
       </c>
-      <c r="G57" s="30" t="n">
+      <c r="G58" s="31" t="n">
         <v>92.67072</v>
       </c>
-      <c r="H57" s="11" t="n">
+      <c r="H58" s="12" t="n">
         <v>83.55507</v>
       </c>
-      <c r="I57" s="30" t="n">
+      <c r="I58" s="31" t="n">
         <v>92.54421000000001</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="inlineStr">
+        <is>
+          <t>PERFORMANCE - MODEL SIZE</t>
+        </is>
+      </c>
+      <c r="B61" s="3" t="n"/>
+      <c r="C61" s="3" t="n"/>
+      <c r="D61" s="3" t="n"/>
+      <c r="E61" s="3" t="n"/>
+      <c r="F61" s="3" t="n"/>
+      <c r="G61" s="3" t="n"/>
+      <c r="H61" s="3" t="n"/>
+      <c r="I61" s="3" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="inlineStr"/>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 20</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 1</t>
+        </is>
+      </c>
+      <c r="D62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 2</t>
+        </is>
+      </c>
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 3</t>
+        </is>
+      </c>
+      <c r="F62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 4</t>
+        </is>
+      </c>
+      <c r="G62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 5</t>
+        </is>
+      </c>
+      <c r="H62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 6</t>
+        </is>
+      </c>
+      <c r="I62" s="1" t="inlineStr">
+        <is>
+          <t>VARIANT 7</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 1 airfoil</t>
+        </is>
+      </c>
+      <c r="B63" s="3" t="n"/>
+      <c r="C63" s="3" t="n"/>
+      <c r="D63" s="3" t="n"/>
+      <c r="E63" s="3" t="n"/>
+      <c r="F63" s="3" t="n"/>
+      <c r="G63" s="3" t="n"/>
+      <c r="H63" s="3" t="n"/>
+      <c r="I63" s="3" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B64" s="105" t="n">
+        <v>36.7</v>
+      </c>
+      <c r="C64" s="106" t="n">
+        <v>35.7</v>
+      </c>
+      <c r="D64" s="107" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="E64" s="108" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="F64" s="109" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G64" s="109" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="H64" s="109" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="I64" s="109" t="n">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B65" s="105" t="n">
+        <v>47</v>
+      </c>
+      <c r="C65" s="110" t="n">
+        <v>45.7</v>
+      </c>
+      <c r="D65" s="111" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="E65" s="112" t="n">
+        <v>41.3</v>
+      </c>
+      <c r="F65" s="109" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="G65" s="113" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="H65" s="109" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="I65" s="114" t="n">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B66" s="105" t="n">
+        <v>62.2</v>
+      </c>
+      <c r="C66" s="115" t="n">
+        <v>68.3</v>
+      </c>
+      <c r="D66" s="116" t="n">
+        <v>68.3</v>
+      </c>
+      <c r="E66" s="117" t="n">
+        <v>58.9</v>
+      </c>
+      <c r="F66" s="118" t="n">
+        <v>59.9</v>
+      </c>
+      <c r="G66" s="119" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="H66" s="120" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="I66" s="119" t="n">
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 2 bike_sharing</t>
+        </is>
+      </c>
+      <c r="B67" s="3" t="n"/>
+      <c r="C67" s="3" t="n"/>
+      <c r="D67" s="3" t="n"/>
+      <c r="E67" s="3" t="n"/>
+      <c r="F67" s="3" t="n"/>
+      <c r="G67" s="3" t="n"/>
+      <c r="H67" s="3" t="n"/>
+      <c r="I67" s="3" t="n"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B68" s="105" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="C68" s="121" t="n">
+        <v>37.3</v>
+      </c>
+      <c r="D68" s="122" t="n">
+        <v>34.1</v>
+      </c>
+      <c r="E68" s="120" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="F68" s="109" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="G68" s="109" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="H68" s="109" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="I68" s="109" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B69" s="105" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="C69" s="123" t="n">
+        <v>44.9</v>
+      </c>
+      <c r="D69" s="118" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="E69" s="124" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="F69" s="125" t="n">
+        <v>29</v>
+      </c>
+      <c r="G69" s="126" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="H69" s="127" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="I69" s="128" t="n">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B70" s="105" t="n">
+        <v>54.9</v>
+      </c>
+      <c r="C70" s="129" t="n">
+        <v>56.1</v>
+      </c>
+      <c r="D70" s="130" t="n">
+        <v>54.1</v>
+      </c>
+      <c r="E70" s="122" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="F70" s="131" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="G70" s="132" t="n">
+        <v>50.7</v>
+      </c>
+      <c r="H70" s="133" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="I70" s="117" t="n">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 3 bioavailability</t>
+        </is>
+      </c>
+      <c r="B71" s="3" t="n"/>
+      <c r="C71" s="3" t="n"/>
+      <c r="D71" s="3" t="n"/>
+      <c r="E71" s="3" t="n"/>
+      <c r="F71" s="3" t="n"/>
+      <c r="G71" s="3" t="n"/>
+      <c r="H71" s="3" t="n"/>
+      <c r="I71" s="3" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B72" s="105" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="C72" s="134" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="D72" s="135" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="E72" s="122" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="F72" s="109" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="G72" s="109" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="H72" s="109" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="I72" s="109" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B73" s="105" t="n">
+        <v>41.6</v>
+      </c>
+      <c r="C73" s="136" t="n">
+        <v>35.4</v>
+      </c>
+      <c r="D73" s="137" t="n">
+        <v>38.1</v>
+      </c>
+      <c r="E73" s="138" t="n">
+        <v>39.8</v>
+      </c>
+      <c r="F73" s="109" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="G73" s="139" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="H73" s="109" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="I73" s="140" t="n">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B74" s="105" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="C74" s="137" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="D74" s="117" t="n">
+        <v>45.9</v>
+      </c>
+      <c r="E74" s="141" t="n">
+        <v>48.1</v>
+      </c>
+      <c r="F74" s="142" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="G74" s="143" t="n">
+        <v>47.7</v>
+      </c>
+      <c r="H74" s="144" t="n">
+        <v>41</v>
+      </c>
+      <c r="I74" s="145" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 5 breast_cancer</t>
+        </is>
+      </c>
+      <c r="B75" s="3" t="n"/>
+      <c r="C75" s="3" t="n"/>
+      <c r="D75" s="3" t="n"/>
+      <c r="E75" s="3" t="n"/>
+      <c r="F75" s="3" t="n"/>
+      <c r="G75" s="3" t="n"/>
+      <c r="H75" s="3" t="n"/>
+      <c r="I75" s="3" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B76" s="105" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="C76" s="146" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="D76" s="146" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="E76" s="147" t="n">
+        <v>25.9</v>
+      </c>
+      <c r="F76" s="109" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G76" s="109" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H76" s="109" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="I76" s="109" t="n">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B77" s="105" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="C77" s="148" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="D77" s="149" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="E77" s="150" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="F77" s="151" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="G77" s="152" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="H77" s="153" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="I77" s="139" t="n">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B78" s="105" t="n">
+        <v>40</v>
+      </c>
+      <c r="C78" s="154" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="D78" s="155" t="n">
+        <v>44.2</v>
+      </c>
+      <c r="E78" s="156" t="n">
+        <v>42.7</v>
+      </c>
+      <c r="F78" s="157" t="n">
+        <v>46.1</v>
+      </c>
+      <c r="G78" s="158" t="n">
+        <v>41.9</v>
+      </c>
+      <c r="H78" s="159" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="I78" s="107" t="n">
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 6 concrete_slump</t>
+        </is>
+      </c>
+      <c r="B79" s="3" t="n"/>
+      <c r="C79" s="3" t="n"/>
+      <c r="D79" s="3" t="n"/>
+      <c r="E79" s="3" t="n"/>
+      <c r="F79" s="3" t="n"/>
+      <c r="G79" s="3" t="n"/>
+      <c r="H79" s="3" t="n"/>
+      <c r="I79" s="3" t="n"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B80" s="105" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="C80" s="160" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="D80" s="161" t="n">
+        <v>30.3</v>
+      </c>
+      <c r="E80" s="129" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="F80" s="109" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G80" s="109" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="H80" s="109" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="I80" s="109" t="n">
+        <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B81" s="105" t="n">
+        <v>40</v>
+      </c>
+      <c r="C81" s="129" t="n">
+        <v>41</v>
+      </c>
+      <c r="D81" s="162" t="n">
+        <v>40.1</v>
+      </c>
+      <c r="E81" s="163" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="F81" s="109" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="G81" s="164" t="n">
+        <v>28</v>
+      </c>
+      <c r="H81" s="109" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="I81" s="165" t="n">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B82" s="105" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="C82" s="166" t="n">
+        <v>56.1</v>
+      </c>
+      <c r="D82" s="156" t="n">
+        <v>57.4</v>
+      </c>
+      <c r="E82" s="156" t="n">
+        <v>57.4</v>
+      </c>
+      <c r="F82" s="163" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="G82" s="167" t="n">
+        <v>51.8</v>
+      </c>
+      <c r="H82" s="105" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="I82" s="119" t="n">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 7 concrete_strength</t>
+        </is>
+      </c>
+      <c r="B83" s="3" t="n"/>
+      <c r="C83" s="3" t="n"/>
+      <c r="D83" s="3" t="n"/>
+      <c r="E83" s="3" t="n"/>
+      <c r="F83" s="3" t="n"/>
+      <c r="G83" s="3" t="n"/>
+      <c r="H83" s="3" t="n"/>
+      <c r="I83" s="3" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B84" s="105" t="n">
+        <v>33.8</v>
+      </c>
+      <c r="C84" s="135" t="n">
+        <v>30.1</v>
+      </c>
+      <c r="D84" s="168" t="n">
+        <v>27.3</v>
+      </c>
+      <c r="E84" s="169" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="F84" s="109" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G84" s="109" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="H84" s="109" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I84" s="109" t="n">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B85" s="105" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="C85" s="124" t="n">
+        <v>39</v>
+      </c>
+      <c r="D85" s="170" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="E85" s="171" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="F85" s="109" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="G85" s="128" t="n">
+        <v>26</v>
+      </c>
+      <c r="H85" s="109" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="I85" s="172" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B86" s="105" t="n">
+        <v>56.3</v>
+      </c>
+      <c r="C86" s="138" t="n">
+        <v>53.9</v>
+      </c>
+      <c r="D86" s="173" t="n">
+        <v>49.7</v>
+      </c>
+      <c r="E86" s="135" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="F86" s="122" t="n">
+        <v>52.7</v>
+      </c>
+      <c r="G86" s="161" t="n">
+        <v>53.2</v>
+      </c>
+      <c r="H86" s="174" t="n">
+        <v>49.3</v>
+      </c>
+      <c r="I86" s="124" t="n">
+        <v>51.1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 8 diabetes</t>
+        </is>
+      </c>
+      <c r="B87" s="3" t="n"/>
+      <c r="C87" s="3" t="n"/>
+      <c r="D87" s="3" t="n"/>
+      <c r="E87" s="3" t="n"/>
+      <c r="F87" s="3" t="n"/>
+      <c r="G87" s="3" t="n"/>
+      <c r="H87" s="3" t="n"/>
+      <c r="I87" s="3" t="n"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B88" s="105" t="n">
+        <v>41.1</v>
+      </c>
+      <c r="C88" s="175" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="D88" s="176" t="n">
+        <v>21.9</v>
+      </c>
+      <c r="E88" s="109" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="F88" s="109" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="G88" s="109" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H88" s="109" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="I88" s="109" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B89" s="105" t="n">
+        <v>51.3</v>
+      </c>
+      <c r="C89" s="177" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="D89" s="178" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="E89" s="109" t="n">
+        <v>24.9</v>
+      </c>
+      <c r="F89" s="109" t="n">
+        <v>19.7</v>
+      </c>
+      <c r="G89" s="109" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="H89" s="109" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="I89" s="109" t="n">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B90" s="105" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="C90" s="117" t="n">
+        <v>59.8</v>
+      </c>
+      <c r="D90" s="179" t="n">
+        <v>46</v>
+      </c>
+      <c r="E90" s="128" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="F90" s="180" t="n">
+        <v>58.1</v>
+      </c>
+      <c r="G90" s="179" t="n">
+        <v>45.9</v>
+      </c>
+      <c r="H90" s="177" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="I90" s="125" t="n">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 9 efficiency_cooling</t>
+        </is>
+      </c>
+      <c r="B91" s="3" t="n"/>
+      <c r="C91" s="3" t="n"/>
+      <c r="D91" s="3" t="n"/>
+      <c r="E91" s="3" t="n"/>
+      <c r="F91" s="3" t="n"/>
+      <c r="G91" s="3" t="n"/>
+      <c r="H91" s="3" t="n"/>
+      <c r="I91" s="3" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B92" s="105" t="n">
+        <v>32.8</v>
+      </c>
+      <c r="C92" s="122" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="D92" s="180" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="E92" s="120" t="n">
+        <v>29.7</v>
+      </c>
+      <c r="F92" s="109" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G92" s="109" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="H92" s="109" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="I92" s="109" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B93" s="105" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="C93" s="161" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="D93" s="122" t="n">
+        <v>38.9</v>
+      </c>
+      <c r="E93" s="120" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="F93" s="109" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="G93" s="181" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="H93" s="109" t="n">
+        <v>13.7</v>
+      </c>
+      <c r="I93" s="109" t="n">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B94" s="105" t="n">
+        <v>53.1</v>
+      </c>
+      <c r="C94" s="182" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="D94" s="107" t="n">
+        <v>54.8</v>
+      </c>
+      <c r="E94" s="107" t="n">
+        <v>54.9</v>
+      </c>
+      <c r="F94" s="175" t="n">
+        <v>47.1</v>
+      </c>
+      <c r="G94" s="183" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="H94" s="184" t="n">
+        <v>45.9</v>
+      </c>
+      <c r="I94" s="185" t="n">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 10 efficiency_heating</t>
+        </is>
+      </c>
+      <c r="B95" s="3" t="n"/>
+      <c r="C95" s="3" t="n"/>
+      <c r="D95" s="3" t="n"/>
+      <c r="E95" s="3" t="n"/>
+      <c r="F95" s="3" t="n"/>
+      <c r="G95" s="3" t="n"/>
+      <c r="H95" s="3" t="n"/>
+      <c r="I95" s="3" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B96" s="105" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="C96" s="133" t="n">
+        <v>32.3</v>
+      </c>
+      <c r="D96" s="161" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="E96" s="120" t="n">
+        <v>28.9</v>
+      </c>
+      <c r="F96" s="109" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G96" s="109" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="H96" s="109" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="I96" s="109" t="n">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B97" s="105" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="C97" s="186" t="n">
+        <v>39.9</v>
+      </c>
+      <c r="D97" s="187" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="E97" s="180" t="n">
+        <v>36.1</v>
+      </c>
+      <c r="F97" s="109" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="G97" s="188" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="H97" s="109" t="n">
+        <v>14.1</v>
+      </c>
+      <c r="I97" s="109" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B98" s="105" t="n">
+        <v>50.9</v>
+      </c>
+      <c r="C98" s="189" t="n">
+        <v>56.4</v>
+      </c>
+      <c r="D98" s="160" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="E98" s="190" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="F98" s="191" t="n">
+        <v>51.2</v>
+      </c>
+      <c r="G98" s="118" t="n">
+        <v>48.9</v>
+      </c>
+      <c r="H98" s="110" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="I98" s="167" t="n">
+        <v>49.1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 11 forest_fires</t>
+        </is>
+      </c>
+      <c r="B99" s="3" t="n"/>
+      <c r="C99" s="3" t="n"/>
+      <c r="D99" s="3" t="n"/>
+      <c r="E99" s="3" t="n"/>
+      <c r="F99" s="3" t="n"/>
+      <c r="G99" s="3" t="n"/>
+      <c r="H99" s="3" t="n"/>
+      <c r="I99" s="3" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B100" s="105" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="C100" s="146" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="D100" s="146" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="E100" s="146" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="F100" s="109" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G100" s="109" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="H100" s="109" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="I100" s="109" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B101" s="105" t="n">
+        <v>29.1</v>
+      </c>
+      <c r="C101" s="192" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="D101" s="193" t="n">
+        <v>36.8</v>
+      </c>
+      <c r="E101" s="194" t="n">
+        <v>39.4</v>
+      </c>
+      <c r="F101" s="195" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="G101" s="196" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="H101" s="197" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="I101" s="196" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B102" s="105" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="C102" s="198" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="D102" s="189" t="n">
+        <v>47.1</v>
+      </c>
+      <c r="E102" s="199" t="n">
+        <v>48.3</v>
+      </c>
+      <c r="F102" s="186" t="n">
+        <v>43.4</v>
+      </c>
+      <c r="G102" s="200" t="n">
+        <v>44.7</v>
+      </c>
+      <c r="H102" s="133" t="n">
+        <v>43</v>
+      </c>
+      <c r="I102" s="200" t="n">
+        <v>44.7</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 12 istanbul</t>
+        </is>
+      </c>
+      <c r="B103" s="3" t="n"/>
+      <c r="C103" s="3" t="n"/>
+      <c r="D103" s="3" t="n"/>
+      <c r="E103" s="3" t="n"/>
+      <c r="F103" s="3" t="n"/>
+      <c r="G103" s="3" t="n"/>
+      <c r="H103" s="3" t="n"/>
+      <c r="I103" s="3" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B104" s="105" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="C104" s="146" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="D104" s="146" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="E104" s="146" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="F104" s="105" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="G104" s="201" t="n">
+        <v>6</v>
+      </c>
+      <c r="H104" s="202" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="I104" s="203" t="n">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B105" s="105" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="C105" s="146" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="D105" s="146" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="E105" s="146" t="n">
+        <v>41.1</v>
+      </c>
+      <c r="F105" s="146" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="G105" s="146" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="H105" s="146" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="I105" s="146" t="n">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B106" s="105" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="C106" s="146" t="n">
+        <v>56.1</v>
+      </c>
+      <c r="D106" s="146" t="n">
+        <v>48.7</v>
+      </c>
+      <c r="E106" s="146" t="n">
+        <v>59.3</v>
+      </c>
+      <c r="F106" s="146" t="n">
+        <v>51.7</v>
+      </c>
+      <c r="G106" s="146" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="H106" s="146" t="n">
+        <v>49.6</v>
+      </c>
+      <c r="I106" s="146" t="n">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 13 parkinson_updrs</t>
+        </is>
+      </c>
+      <c r="B107" s="3" t="n"/>
+      <c r="C107" s="3" t="n"/>
+      <c r="D107" s="3" t="n"/>
+      <c r="E107" s="3" t="n"/>
+      <c r="F107" s="3" t="n"/>
+      <c r="G107" s="3" t="n"/>
+      <c r="H107" s="3" t="n"/>
+      <c r="I107" s="3" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B108" s="105" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="C108" s="204" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="D108" s="205" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="E108" s="175" t="n">
+        <v>31.3</v>
+      </c>
+      <c r="F108" s="109" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G108" s="109" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="H108" s="109" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="I108" s="109" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B109" s="105" t="n">
+        <v>42.1</v>
+      </c>
+      <c r="C109" s="206" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="D109" s="162" t="n">
+        <v>42.2</v>
+      </c>
+      <c r="E109" s="137" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="F109" s="109" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="G109" s="207" t="n">
+        <v>25.7</v>
+      </c>
+      <c r="H109" s="109" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="I109" s="207" t="n">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B110" s="105" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="C110" s="208" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="D110" s="129" t="n">
+        <v>54.5</v>
+      </c>
+      <c r="E110" s="145" t="n">
+        <v>51.7</v>
+      </c>
+      <c r="F110" s="144" t="n">
+        <v>45.1</v>
+      </c>
+      <c r="G110" s="161" t="n">
+        <v>50.3</v>
+      </c>
+      <c r="H110" s="209" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="I110" s="122" t="n">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 14 ppb</t>
+        </is>
+      </c>
+      <c r="B111" s="3" t="n"/>
+      <c r="C111" s="3" t="n"/>
+      <c r="D111" s="3" t="n"/>
+      <c r="E111" s="3" t="n"/>
+      <c r="F111" s="3" t="n"/>
+      <c r="G111" s="3" t="n"/>
+      <c r="H111" s="3" t="n"/>
+      <c r="I111" s="3" t="n"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B112" s="105" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="C112" s="210" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="D112" s="183" t="n">
+        <v>29</v>
+      </c>
+      <c r="E112" s="112" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="F112" s="109" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="G112" s="109" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="H112" s="109" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="I112" s="109" t="n">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B113" s="105" t="n">
+        <v>35.2</v>
+      </c>
+      <c r="C113" s="211" t="n">
+        <v>37.8</v>
+      </c>
+      <c r="D113" s="186" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="E113" s="185" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="F113" s="109" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="G113" s="114" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="H113" s="109" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="I113" s="212" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B114" s="105" t="n">
+        <v>42.6</v>
+      </c>
+      <c r="C114" s="111" t="n">
+        <v>45.7</v>
+      </c>
+      <c r="D114" s="213" t="n">
+        <v>43.4</v>
+      </c>
+      <c r="E114" s="167" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="F114" s="185" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="G114" s="191" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="H114" s="185" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="I114" s="187" t="n">
+        <v>42.8</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="4" t="inlineStr">
+        <is>
+          <t>Dataset 15 resid_build_sale_price</t>
+        </is>
+      </c>
+      <c r="B115" s="3" t="n"/>
+      <c r="C115" s="3" t="n"/>
+      <c r="D115" s="3" t="n"/>
+      <c r="E115" s="3" t="n"/>
+      <c r="F115" s="3" t="n"/>
+      <c r="G115" s="3" t="n"/>
+      <c r="H115" s="3" t="n"/>
+      <c r="I115" s="3" t="n"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="5" t="inlineStr">
+        <is>
+          <t>Smallest</t>
+        </is>
+      </c>
+      <c r="B116" s="105" t="n">
+        <v>29</v>
+      </c>
+      <c r="C116" s="120" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="D116" s="182" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="E116" s="180" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="F116" s="109" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G116" s="109" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="H116" s="109" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="I116" s="109" t="n">
+        <v>8.300000000000001</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="5" t="inlineStr">
+        <is>
+          <t>Best normalized</t>
+        </is>
+      </c>
+      <c r="B117" s="105" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="C117" s="202" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="D117" s="205" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="E117" s="119" t="n">
+        <v>33.1</v>
+      </c>
+      <c r="F117" s="109" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="G117" s="214" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="H117" s="109" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="I117" s="215" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="5" t="inlineStr">
+        <is>
+          <t>Best fitness</t>
+        </is>
+      </c>
+      <c r="B118" s="105" t="n">
+        <v>42.3</v>
+      </c>
+      <c r="C118" s="167" t="n">
+        <v>40.9</v>
+      </c>
+      <c r="D118" s="160" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="E118" s="118" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="F118" s="185" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="G118" s="167" t="n">
+        <v>40.9</v>
+      </c>
+      <c r="H118" s="185" t="n">
+        <v>39.4</v>
+      </c>
+      <c r="I118" s="205" t="n">
+        <v>41.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>